<commit_message>
New Login User flow fix
</commit_message>
<xml_diff>
--- a/ConfigFile.xlsx
+++ b/ConfigFile.xlsx
@@ -1,111 +1,162 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sangeetha.a\Documents\UiPath\TransactionalPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07A2079-57FE-4EDA-BBB5-8A058FC78AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="5" r:id="rId2"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>portal.azure.com</t>
-  </si>
-  <si>
-    <t>URL Description</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>portal.azure.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL Description</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CP-FSM-DT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CP-FSM-PROD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>crisplantdev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crisplantfsmdev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GosigerDev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IFSDT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IFSPROD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>imaxdev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RACQ</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color theme="10"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="5">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,87 +421,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="19" style="3" customWidth="1"/>
+    <x:col min="2" max="2" width="37.140625" style="3" customWidth="1"/>
+    <x:col min="3" max="3" width="42.425781" style="3" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="3" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="3" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="B3" s="4" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="B4" s="4" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A9"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Login page combination validation fix
</commit_message>
<xml_diff>
--- a/ConfigFile.xlsx
+++ b/ConfigFile.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sangeetha.a\Documents\UiPath\TransactionalPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07A2079-57FE-4EDA-BBB5-8A058FC78AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509C287C-C38A-4888-8784-4DA2D514524B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <x:sheet name="Sheet2" sheetId="5" r:id="rId2"/>
+    <x:sheet name="Sheet3" sheetId="6" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -27,7 +28,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <x:si>
+    <x:t>Server Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Crisplantfsmdev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9.74 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.18 /s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RACQ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8.24 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.71 /s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GosigerDev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7.58 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51.04 /s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IFSDT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9.44 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6.74 /s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IFSPROD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.46 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4.15 /s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>imaxdev</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7.48 MB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0.19 /s</x:t>
+  </x:si>
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -54,24 +112,6 @@
   </x:si>
   <x:si>
     <x:t>crisplantdev</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Crisplantfsmdev</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GosigerDev</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IFSDT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IFSPROD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>imaxdev</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RACQ</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -122,20 +162,45 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="18" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -421,48 +486,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{61D97514-0DED-4F3F-BE7F-EB4EF3458179}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:G7"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A2" sqref="A2 A2:A2"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="15.570312" style="7" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="7" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="10" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B2" s="8" t="n">
+        <x:v>0.0753</x:v>
+      </x:c>
+      <x:c r="C2" s="9" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D2" s="9" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E2" s="9" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F2" s="9" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="G2" s="9" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="7" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="8" t="n">
+        <x:v>0.4997</x:v>
+      </x:c>
+      <x:c r="C3" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D3" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E3" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F3" s="7" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="G3" s="7" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="7" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B4" s="8" t="n">
+        <x:v>0.1853</x:v>
+      </x:c>
+      <x:c r="C4" s="7" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D4" s="7" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="7" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F4" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G4" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="7" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B5" s="8" t="n">
+        <x:v>0.2845</x:v>
+      </x:c>
+      <x:c r="C5" s="7" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D5" s="7" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E5" s="7" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F5" s="7" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G5" s="7" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="7" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B6" s="8" t="n">
+        <x:v>0.0032</x:v>
+      </x:c>
+      <x:c r="C6" s="7" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D6" s="7" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E6" s="7" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F6" s="7" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G6" s="7" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="7" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B7" s="8" t="n">
+        <x:v>0.0064</x:v>
+      </x:c>
+      <x:c r="C7" s="7" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D7" s="7" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E7" s="7" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F7" s="7" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="G7" s="7" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="A7" r:id="rId12"/>
+    <x:hyperlink ref="A6" r:id="rId13"/>
+    <x:hyperlink ref="A5" r:id="rId14"/>
+    <x:hyperlink ref="A2" r:id="rId15"/>
+    <x:hyperlink ref="A4" r:id="rId16"/>
+  </x:hyperlinks>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:C4"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="19" style="3" customWidth="1"/>
-    <x:col min="2" max="2" width="37.140625" style="3" customWidth="1"/>
-    <x:col min="3" max="3" width="42.425781" style="3" customWidth="1"/>
+    <x:col min="1" max="1" width="19" style="7" customWidth="1"/>
+    <x:col min="2" max="2" width="37.140625" style="7" customWidth="1"/>
+    <x:col min="3" max="3" width="42.425781" style="7" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="3" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="3" t="s">
-        <x:v>2</x:v>
+      <x:c r="A1" s="7" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B1" s="7" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C1" s="7" t="s">
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="3" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B2" s="3" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="3" t="s">
-        <x:v>5</x:v>
+      <x:c r="A2" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B2" s="7" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C2" s="7" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="B3" s="4" t="s"/>
+      <x:c r="B3" s="11" t="s"/>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="B4" s="4" t="s"/>
+      <x:c r="B4" s="11" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -473,7 +714,7 @@
 </x:worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
@@ -485,48 +726,48 @@
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="3" t="s">
-        <x:v>6</x:v>
+      <x:c r="A1" s="7" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="3" t="s">
+      <x:c r="A2" s="7" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="7" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="7" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="3" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="3" t="s">
+    <x:row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="7" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
     <x:row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="3" t="s">
-        <x:v>12</x:v>
+      <x:c r="A7" s="7" t="s">
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="3" t="s">
-        <x:v>13</x:v>
+      <x:c r="A8" s="7" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="3" t="s">
-        <x:v>14</x:v>
+      <x:c r="A9" s="7" t="s">
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Updated Code(Write sequence combined under 1 flow) - 040220
</commit_message>
<xml_diff>
--- a/ConfigFile.xlsx
+++ b/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sangeetha.a\Documents\UiPath\TransactionalPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0852F23A-FF01-4DD9-A1C4-B99A2FB3CF13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9872F5-327A-45D8-ADFE-4EE34297ED87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -109,12 +109,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
     <t>CP-FSM-DT</t>
   </si>
   <si>
@@ -133,130 +127,214 @@
     <t>RACQ</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>61.65 MB</t>
+  </si>
+  <si>
+    <t>130.85 MB</t>
+  </si>
+  <si>
+    <t>95.15 MB</t>
+  </si>
+  <si>
+    <t>285.27 MB</t>
+  </si>
+  <si>
+    <t>0.13 /s</t>
+  </si>
+  <si>
+    <t>4.26 /s</t>
+  </si>
+  <si>
+    <t>10.39 MB</t>
+  </si>
+  <si>
+    <t>30.59 MB</t>
+  </si>
+  <si>
+    <t>16.75 GB</t>
+  </si>
+  <si>
+    <t>81.74 GB</t>
+  </si>
+  <si>
+    <t>80.21 /s</t>
+  </si>
+  <si>
+    <t>446.43 /s</t>
+  </si>
+  <si>
     <t>Stop</t>
   </si>
   <si>
-    <t>8.76 MB</t>
-  </si>
-  <si>
-    <t>3.07 /s</t>
-  </si>
-  <si>
-    <t>10.08 /s</t>
-  </si>
-  <si>
-    <t>2.52 /s</t>
-  </si>
-  <si>
-    <t>Disk Read Bytes (Sum)Disk Read Bytes (Sum)Disk Read Bytes (Sum)ifsprodifsprodifsprod6.34 GBDisk Write Bytes (Sum)Disk Write Bytes (Sum)Disk Write Bytes (Sum)ifsprodifsprodifsprod457.73 MB</t>
-  </si>
-  <si>
-    <t>457.73 MB</t>
-  </si>
-  <si>
-    <t>6.34 GB</t>
-  </si>
-  <si>
-    <t>215.69 /s</t>
-  </si>
-  <si>
-    <t>28.19 MB</t>
-  </si>
-  <si>
-    <t>302.4 MB</t>
-  </si>
-  <si>
-    <t>467.74 MB</t>
-  </si>
-  <si>
-    <t>0.17 /s</t>
-  </si>
-  <si>
-    <t>5.24 MB</t>
-  </si>
-  <si>
-    <t>18.96 MB</t>
-  </si>
-  <si>
-    <t>275.99 MB</t>
-  </si>
-  <si>
-    <t>438.28 MB</t>
-  </si>
-  <si>
-    <t>0.63 /s</t>
-  </si>
-  <si>
-    <t>17.39 MB</t>
-  </si>
-  <si>
-    <t>64.53 MB</t>
-  </si>
-  <si>
-    <t>48.52 MB</t>
-  </si>
-  <si>
-    <t>288.13 MB</t>
-  </si>
-  <si>
-    <t>0.06 /s</t>
-  </si>
-  <si>
-    <t>3.99 /s</t>
-  </si>
-  <si>
-    <t>22.64 MB</t>
-  </si>
-  <si>
-    <t>65.54 MB</t>
-  </si>
-  <si>
-    <t>48.51 MB</t>
-  </si>
-  <si>
-    <t>288.31 MB</t>
-  </si>
-  <si>
-    <t>0.05 /s</t>
-  </si>
-  <si>
-    <t>4 /s</t>
-  </si>
-  <si>
-    <t>8.79 MB</t>
-  </si>
-  <si>
-    <t>28.56 MB</t>
-  </si>
-  <si>
-    <t>17.67 GB</t>
-  </si>
-  <si>
-    <t>81.24 GB</t>
-  </si>
-  <si>
-    <t>118.5 /s</t>
-  </si>
-  <si>
-    <t>409.79 /s</t>
-  </si>
-  <si>
-    <t>8.45 MB</t>
-  </si>
-  <si>
-    <t>8.2 MB</t>
-  </si>
-  <si>
-    <t>470.33 MB</t>
-  </si>
-  <si>
-    <t>878.86 MB</t>
-  </si>
-  <si>
-    <t>6.91 /s</t>
-  </si>
-  <si>
-    <t>16.73 /s</t>
+    <t>6.26 MB</t>
+  </si>
+  <si>
+    <t>5.83 MB</t>
+  </si>
+  <si>
+    <t>474.27 MB</t>
+  </si>
+  <si>
+    <t>926.79 MB</t>
+  </si>
+  <si>
+    <t>6.88 /s</t>
+  </si>
+  <si>
+    <t>17.01 /s</t>
+  </si>
+  <si>
+    <t>3.32 MB</t>
+  </si>
+  <si>
+    <t>1.35 MB</t>
+  </si>
+  <si>
+    <t>7.21 GB</t>
+  </si>
+  <si>
+    <t>572.6 MB</t>
+  </si>
+  <si>
+    <t>241.78 /s</t>
+  </si>
+  <si>
+    <t>10.29 /s</t>
+  </si>
+  <si>
+    <t>15.46 MB</t>
+  </si>
+  <si>
+    <t>28.52 MB</t>
+  </si>
+  <si>
+    <t>343.46 MB</t>
+  </si>
+  <si>
+    <t>745.15 MB</t>
+  </si>
+  <si>
+    <t>0.45 /s</t>
+  </si>
+  <si>
+    <t>3.42 /s</t>
+  </si>
+  <si>
+    <t>4.71 MB</t>
+  </si>
+  <si>
+    <t>17.89 MB</t>
+  </si>
+  <si>
+    <t>275.08 MB</t>
+  </si>
+  <si>
+    <t>426.97 MB</t>
+  </si>
+  <si>
+    <t>0.7 /s</t>
+  </si>
+  <si>
+    <t>2.97 /s</t>
+  </si>
+  <si>
+    <t>60.59 MB</t>
+  </si>
+  <si>
+    <t>128.66 MB</t>
+  </si>
+  <si>
+    <t>97.27 MB</t>
+  </si>
+  <si>
+    <t>289.73 MB</t>
+  </si>
+  <si>
+    <t>4.29 /s</t>
+  </si>
+  <si>
+    <t>10.44 MB</t>
+  </si>
+  <si>
+    <t>30.63 MB</t>
+  </si>
+  <si>
+    <t>16.72 GB</t>
+  </si>
+  <si>
+    <t>80.62 GB</t>
+  </si>
+  <si>
+    <t>81.6 /s</t>
+  </si>
+  <si>
+    <t>444.77 /s</t>
+  </si>
+  <si>
+    <t>6.31 MB</t>
+  </si>
+  <si>
+    <t>5.88 MB</t>
+  </si>
+  <si>
+    <t>467.3 MB</t>
+  </si>
+  <si>
+    <t>921.52 MB</t>
+  </si>
+  <si>
+    <t>6.9 /s</t>
+  </si>
+  <si>
+    <t>17.03 /s</t>
+  </si>
+  <si>
+    <t>3.33 MB</t>
+  </si>
+  <si>
+    <t>7.15 GB</t>
+  </si>
+  <si>
+    <t>567.49 MB</t>
+  </si>
+  <si>
+    <t>239.65 /s</t>
+  </si>
+  <si>
+    <t>10.26 /s</t>
+  </si>
+  <si>
+    <t>14.93 MB</t>
+  </si>
+  <si>
+    <t>28.4 MB</t>
+  </si>
+  <si>
+    <t>337.85 MB</t>
+  </si>
+  <si>
+    <t>740.35 MB</t>
+  </si>
+  <si>
+    <t>0.44 /s</t>
+  </si>
+  <si>
+    <t>3.38 /s</t>
+  </si>
+  <si>
+    <t>4.72 MB</t>
+  </si>
+  <si>
+    <t>17.9 MB</t>
+  </si>
+  <si>
+    <t>426.78 MB</t>
+  </si>
+  <si>
+    <t>2.98 /s</t>
   </si>
 </sst>
 </file>
@@ -328,13 +406,23 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -345,6 +433,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{715A8EF6-A505-4210-B066-D832C9256031}" name="Table1" displayName="Table1" ref="A1:L81" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:L81" xr:uid="{55C6404D-BE9A-4778-95AA-177B65E9707E}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{9A7B1D62-DD64-4DB1-B5F6-3158A1BFBBD2}" name="Server_Name"/>
+    <tableColumn id="2" xr3:uid="{E38D28C9-32E7-42D2-8010-278DF4ACA222}" name="Server_Status"/>
+    <tableColumn id="3" xr3:uid="{D9F0E434-2358-4093-AB0E-5A3B294D9EF5}" name="CPU Utilization" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{06F24F33-243B-4453-B923-C5C36813A3F5}" name="NetworkInTotal"/>
+    <tableColumn id="5" xr3:uid="{280257BE-CCA6-4CEF-9A0A-ABB95616AA9C}" name="NetworkOutTotal"/>
+    <tableColumn id="6" xr3:uid="{90A450DF-4F86-4836-B83F-C18E0B0D4DA7}" name="Disk Bytes_Read value"/>
+    <tableColumn id="7" xr3:uid="{6988EAE1-FBDE-492D-A21F-B4530A75A227}" name="Disk Bytes_Write value"/>
+    <tableColumn id="8" xr3:uid="{7B53895D-E29E-41A3-8C9A-B3E040444952}" name="Disk Operation_Read value"/>
+    <tableColumn id="9" xr3:uid="{DFCD698E-0789-4746-9289-53CD5484BE1C}" name="Disk Operation_Write value"/>
+    <tableColumn id="10" xr3:uid="{C56B5794-A865-4171-A46F-77AA07519B21}" name="Checked At" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{0BC98B91-BA1B-45CE-9DB5-B6BFDBECD97B}" name="Status"/>
+    <tableColumn id="12" xr3:uid="{D4846CB1-A5B2-4D42-BD29-57A320C3362E}" name="Threshold_Limit"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -610,11 +719,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83B3495-1552-4419-820B-A97AC3E82D33}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -651,7 +758,7 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="D2" s="8">
-        <v>43864.637291666666</v>
+        <v>43865.422372685185</v>
       </c>
       <c r="E2" t="s">
         <v>24</v>
@@ -669,7 +776,7 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="D3" s="8">
-        <v>43864.637326388889</v>
+        <v>43865.422523148147</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -687,7 +794,7 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="D4" s="8">
-        <v>43864.637326388889</v>
+        <v>43865.422546296293</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -705,7 +812,7 @@
         <v>7.2300000000000003E-2</v>
       </c>
       <c r="D5" s="8">
-        <v>43864.637337962966</v>
+        <v>43865.42255787037</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -720,14 +827,9 @@
         <v>19</v>
       </c>
       <c r="C6" s="7">
-        <v>7.2300000000000003E-2</v>
-      </c>
-      <c r="D6" s="8">
-        <v>43864.637361111112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
+        <v>7.6E-3</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,93 +838,28 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D8" s="8">
-        <v>43864.637372685182</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D9" s="8">
-        <v>43864.637372685182</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D10" s="8">
-        <v>43864.637384259258</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D11" s="8">
-        <v>43864.637384259258</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D12" s="8">
-        <v>43864.637384259258</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -831,118 +868,173 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D14" s="8">
-        <v>43864.637395833335</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D15" s="8">
-        <v>43864.637407407405</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D16" s="8">
-        <v>43864.637407407405</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D17" s="8">
-        <v>43864.637418981481</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="7">
-        <v>8.2299999999999998E-2</v>
-      </c>
-      <c r="D18" s="8">
-        <v>43864.637418981481</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
       <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="7"/>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="7"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="7"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="7"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="7"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="D52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1043,55 +1135,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964FAE33-6CD9-4087-B134-2594D9E9DD3D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>7.3700000000000002E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>0.13300000000000001</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1100,14 +1149,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0904079-205D-45A4-AC1C-11F8F03898FC}">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1150,10 +1207,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="8">
+        <v>43865.461342592593</v>
       </c>
       <c r="L2" s="5">
         <v>0.1</v>
@@ -1161,10 +1242,34 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="8">
+        <v>43865.461354166669</v>
       </c>
       <c r="L3" s="5">
         <v>0.1</v>
@@ -1172,10 +1277,34 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="8">
+        <v>43865.461365740739</v>
       </c>
       <c r="L4" s="5">
         <v>0.1</v>
@@ -1183,10 +1312,34 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="8">
+        <v>43865.461388888885</v>
       </c>
       <c r="L5" s="5">
         <v>0.1</v>
@@ -1200,28 +1353,28 @@
         <v>19</v>
       </c>
       <c r="C6" s="7">
-        <v>7.8200000000000006E-2</v>
+        <v>8.9399999999999993E-2</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="J6" s="8">
-        <v>43864.734155092592</v>
+        <v>43865.461458333331</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>24</v>
@@ -1238,31 +1391,31 @@
         <v>19</v>
       </c>
       <c r="C7" s="7">
-        <v>0.17749999999999999</v>
+        <v>0.16889999999999999</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="J7" s="8">
-        <v>43864.734363425923</v>
+        <v>43865.461585648147</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L7" s="5">
         <v>0.1</v>
@@ -1276,31 +1429,31 @@
         <v>19</v>
       </c>
       <c r="C8" s="7">
-        <v>0.27710000000000001</v>
+        <v>0.26069999999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="J8" s="8">
-        <v>43864.734826388885</v>
+        <v>43865.461701388886</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L8" s="5">
         <v>0.1</v>
@@ -1314,28 +1467,28 @@
         <v>19</v>
       </c>
       <c r="C9" s="7">
-        <v>3.8399999999999997E-2</v>
+        <v>4.19E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J9" s="8">
-        <v>43864.729166666664</v>
+        <v>43865.461817129632</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>24</v>
@@ -1352,28 +1505,28 @@
         <v>19</v>
       </c>
       <c r="C10" s="7">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="J10" s="8">
-        <v>43864.729305555556</v>
+        <v>43865.46193287037</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>24</v>
@@ -1384,37 +1537,37 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7">
-        <v>0.49790000000000001</v>
+        <v>0.49740000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="I11" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="J11" s="8">
-        <v>43864.729444444441</v>
+        <v>43865.462048611109</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="L11" s="5">
         <v>0.1</v>
@@ -1422,44 +1575,144 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="8">
+        <v>43865.462106481478</v>
+      </c>
+      <c r="K12" s="8"/>
       <c r="L12" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="8">
+        <v>43865.462129629632</v>
+      </c>
+      <c r="K13" s="8"/>
       <c r="L13" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="8">
+        <v>43865.462141203701</v>
+      </c>
+      <c r="K14" s="8"/>
       <c r="L14" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="8">
+        <v>43865.462152777778</v>
+      </c>
+      <c r="K15" s="8"/>
       <c r="L15" s="5">
         <v>0.1</v>
       </c>
@@ -1472,28 +1725,28 @@
         <v>19</v>
       </c>
       <c r="C16" s="7">
-        <v>8.2500000000000004E-2</v>
+        <v>8.9499999999999996E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="J16" s="8">
-        <v>43864.729583333334</v>
+        <v>43865.462222222224</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>24</v>
@@ -1509,9 +1762,33 @@
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="10"/>
+      <c r="C17" s="7">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="8">
+        <v>43865.462337962963</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="L17" s="5">
         <v>0.1</v>
       </c>
@@ -1523,9 +1800,33 @@
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="10"/>
+      <c r="C18" s="7">
+        <v>0.26090000000000002</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="8">
+        <v>43865.462465277778</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="L18" s="5">
         <v>0.1</v>
       </c>
@@ -1537,9 +1838,33 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9"/>
+      <c r="C19" s="7">
+        <v>4.1799999999999997E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="8">
+        <v>43865.462569444448</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="L19" s="5">
         <v>0.1</v>
       </c>
@@ -1551,359 +1876,430 @@
       <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="9"/>
+      <c r="C20" s="7">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="8">
+        <v>43865.462685185186</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="L20" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="10"/>
+      <c r="C21" s="7">
+        <v>0.49740000000000001</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="8">
+        <v>43865.462800925925</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="L21" s="5">
         <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K22" s="8"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K23" s="8"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24" s="8"/>
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" s="8"/>
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="10"/>
+      <c r="K26" s="8"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="J27" s="8"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="8"/>
       <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C28" s="7"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="10"/>
+      <c r="K28" s="8"/>
       <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C29" s="7"/>
       <c r="J29" s="8"/>
-      <c r="K29" s="9"/>
+      <c r="K29" s="8"/>
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C30" s="7"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="9"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" s="7"/>
       <c r="J31" s="8"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="8"/>
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32" s="8"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K33" s="8"/>
       <c r="L33" s="5"/>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K34" s="8"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="8"/>
       <c r="L35" s="5"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C36" s="7"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="10"/>
+      <c r="K36" s="8"/>
       <c r="L36" s="5"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C37" s="5"/>
       <c r="J37" s="8"/>
-      <c r="K37" s="10"/>
+      <c r="K37" s="8"/>
       <c r="L37" s="5"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="10"/>
+      <c r="K38" s="8"/>
       <c r="L38" s="5"/>
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C39" s="7"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="9"/>
+      <c r="K39" s="8"/>
       <c r="L39" s="5"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C40" s="7"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="9"/>
+      <c r="K40" s="8"/>
       <c r="L40" s="5"/>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C41" s="7"/>
       <c r="J41" s="8"/>
-      <c r="K41" s="10"/>
+      <c r="K41" s="8"/>
       <c r="L41" s="5"/>
     </row>
     <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K42" s="8"/>
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K43" s="8"/>
       <c r="L43" s="5"/>
     </row>
     <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K44" s="8"/>
       <c r="L44" s="5"/>
     </row>
     <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K45" s="8"/>
       <c r="L45" s="5"/>
     </row>
     <row r="46" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C46" s="7"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="10"/>
+      <c r="K46" s="8"/>
       <c r="L46" s="5"/>
     </row>
     <row r="47" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C47" s="7"/>
       <c r="J47" s="8"/>
-      <c r="K47" s="10"/>
+      <c r="K47" s="8"/>
       <c r="L47" s="5"/>
     </row>
     <row r="48" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C48" s="7"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="10"/>
+      <c r="K48" s="8"/>
       <c r="L48" s="5"/>
     </row>
     <row r="49" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="J49" s="8"/>
-      <c r="K49" s="9"/>
+      <c r="K49" s="8"/>
       <c r="L49" s="5"/>
     </row>
     <row r="50" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="9"/>
+      <c r="K50" s="8"/>
       <c r="L50" s="5"/>
     </row>
     <row r="51" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C51" s="7"/>
       <c r="J51" s="8"/>
-      <c r="K51" s="10"/>
+      <c r="K51" s="8"/>
       <c r="L51" s="5"/>
     </row>
     <row r="52" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K52" s="8"/>
       <c r="L52" s="5"/>
     </row>
     <row r="53" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K53" s="8"/>
       <c r="L53" s="5"/>
     </row>
     <row r="54" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K54" s="8"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K55" s="8"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C56" s="7"/>
       <c r="J56" s="8"/>
-      <c r="K56" s="10"/>
+      <c r="K56" s="8"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C57" s="7"/>
       <c r="J57" s="8"/>
-      <c r="K57" s="10"/>
+      <c r="K57" s="8"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C58" s="7"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="10"/>
+      <c r="K58" s="8"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C59" s="7"/>
       <c r="J59" s="8"/>
-      <c r="K59" s="9"/>
+      <c r="K59" s="8"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C60" s="7"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="9"/>
+      <c r="K60" s="8"/>
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C61" s="7"/>
       <c r="J61" s="8"/>
-      <c r="K61" s="10"/>
+      <c r="K61" s="8"/>
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K62" s="8"/>
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K63" s="8"/>
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K64" s="8"/>
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K65" s="8"/>
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C66" s="7"/>
       <c r="J66" s="8"/>
-      <c r="K66" s="10"/>
+      <c r="K66" s="8"/>
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="J67" s="8"/>
-      <c r="K67" s="10"/>
+      <c r="K67" s="8"/>
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C68" s="7"/>
       <c r="J68" s="8"/>
-      <c r="K68" s="10"/>
+      <c r="K68" s="8"/>
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C69" s="7"/>
       <c r="J69" s="8"/>
-      <c r="K69" s="9"/>
+      <c r="K69" s="8"/>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C70" s="7"/>
       <c r="J70" s="8"/>
-      <c r="K70" s="9"/>
+      <c r="K70" s="8"/>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C71" s="7"/>
       <c r="J71" s="8"/>
-      <c r="K71" s="10"/>
+      <c r="K71" s="8"/>
       <c r="L71" s="5"/>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K72" s="8"/>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K73" s="8"/>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K74" s="8"/>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="K75" s="8"/>
     </row>
     <row r="76" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="J76" s="8"/>
-      <c r="K76" s="10"/>
+      <c r="K76" s="8"/>
     </row>
     <row r="77" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C77" s="7"/>
       <c r="J77" s="8"/>
-      <c r="K77" s="10"/>
+      <c r="K77" s="8"/>
     </row>
     <row r="78" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C78" s="7"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="10"/>
+      <c r="K78" s="8"/>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C79" s="7"/>
       <c r="J79" s="8"/>
-      <c r="K79" s="9"/>
+      <c r="K79" s="8"/>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C80" s="7"/>
       <c r="J80" s="8"/>
-      <c r="K80" s="9"/>
+      <c r="K80" s="8"/>
     </row>
     <row r="81" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C81" s="7"/>
       <c r="J81" s="8"/>
-      <c r="K81" s="10"/>
+      <c r="K81" s="8"/>
     </row>
     <row r="86" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C86" s="7"/>
       <c r="J86" s="8"/>
-      <c r="K86" s="10"/>
     </row>
     <row r="87" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C87" s="7"/>
       <c r="J87" s="8"/>
-      <c r="K87" s="10"/>
     </row>
     <row r="88" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C88" s="7"/>
       <c r="J88" s="8"/>
-      <c r="K88" s="10"/>
     </row>
     <row r="89" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C89" s="7"/>
       <c r="J89" s="8"/>
-      <c r="K89" s="9"/>
     </row>
     <row r="90" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C90" s="7"/>
       <c r="J90" s="8"/>
-      <c r="K90" s="9"/>
     </row>
     <row r="91" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C91" s="7"/>
       <c r="J91" s="8"/>
-      <c r="K91" s="10"/>
     </row>
     <row r="96" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C96" s="7"/>
       <c r="J96" s="8"/>
-      <c r="K96" s="10"/>
-    </row>
-    <row r="97" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C97" s="7"/>
       <c r="J97" s="8"/>
-      <c r="K97" s="10"/>
-    </row>
-    <row r="98" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C98" s="7"/>
       <c r="J98" s="8"/>
-      <c r="K98" s="10"/>
-    </row>
-    <row r="99" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C99" s="7"/>
       <c r="J99" s="8"/>
-      <c r="K99" s="9"/>
-    </row>
-    <row r="100" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
       <c r="J100" s="8"/>
-      <c r="K100" s="9"/>
-    </row>
-    <row r="101" spans="3:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C101" s="7"/>
       <c r="J101" s="8"/>
-      <c r="K101" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>